<commit_message>
Add 2 spreadsheet to sync-* docs
</commit_message>
<xml_diff>
--- a/_book/offline/assets/watch-1b.xlsx
+++ b/_book/offline/assets/watch-1b.xlsx
@@ -421,15 +421,6 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -448,6 +439,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -747,17 +747,17 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="28" t="s">
         <v>19</v>
       </c>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="22"/>
-      <c r="F2" s="20" t="s">
+      <c r="C2" s="29"/>
+      <c r="D2" s="29"/>
+      <c r="E2" s="30"/>
+      <c r="F2" s="28" t="s">
         <v>20</v>
       </c>
-      <c r="G2" s="21"/>
-      <c r="H2" s="22"/>
+      <c r="G2" s="29"/>
+      <c r="H2" s="30"/>
     </row>
     <row r="3" spans="2:8" s="1" customFormat="1" ht="30" x14ac:dyDescent="0.25">
       <c r="B3" s="5" t="s">
@@ -807,7 +807,7 @@
       <c r="B5" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C5" s="29" t="s">
+      <c r="C5" s="26" t="s">
         <v>6</v>
       </c>
       <c r="D5" s="11">
@@ -816,36 +816,36 @@
       <c r="E5" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="F5" s="30" t="s">
+      <c r="F5" s="27" t="s">
         <v>5</v>
       </c>
-      <c r="G5" s="29" t="s">
+      <c r="G5" s="26" t="s">
         <v>11</v>
       </c>
       <c r="H5" s="13" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="6" spans="2:8" s="28" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B6" s="23" t="s">
+    <row r="6" spans="2:8" s="25" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B6" s="20" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="21" t="s">
         <v>10</v>
       </c>
-      <c r="D6" s="25">
+      <c r="D6" s="22">
         <v>0.71180555555555547</v>
       </c>
-      <c r="E6" s="26" t="s">
+      <c r="E6" s="23" t="s">
         <v>13</v>
       </c>
-      <c r="F6" s="27" t="s">
+      <c r="F6" s="24" t="s">
         <v>10</v>
       </c>
-      <c r="G6" s="24" t="s">
+      <c r="G6" s="21" t="s">
         <v>11</v>
       </c>
-      <c r="H6" s="24" t="s">
+      <c r="H6" s="21" t="s">
         <v>14</v>
       </c>
     </row>

</xml_diff>